<commit_message>
modified some variable name
</commit_message>
<xml_diff>
--- a/bin/testdata/forgotpassTestdata.xlsx
+++ b/bin/testdata/forgotpassTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FC6F7-C098-4F0C-9612-AC374B82E97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5967BF4D-974B-407C-BD00-48799489EE6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" xr2:uid="{A67994D8-9304-4902-8656-C43FCA99F059}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>confirmpass</t>
   </si>
   <si>
-    <t>remark</t>
-  </si>
-  <si>
     <t>wk@g.com</t>
   </si>
   <si>
@@ -76,13 +73,16 @@
   </si>
   <si>
     <t>Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +98,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,9 +134,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,80 +456,83 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1234567890</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,5 +547,6 @@
     <hyperlink ref="D4" r:id="rId8" xr:uid="{B5D0C938-B63F-4D45-92EF-28F7641288FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added .gitignore file at root level
</commit_message>
<xml_diff>
--- a/bin/testdata/forgotpassTestdata.xlsx
+++ b/bin/testdata/forgotpassTestdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shivam_kushwaha\eclipse-workspace\ShoppingPortal\src\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0FC6F7-C098-4F0C-9612-AC374B82E97E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5967BF4D-974B-407C-BD00-48799489EE6D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2200" yWindow="2200" windowWidth="14400" windowHeight="7360" xr2:uid="{A67994D8-9304-4902-8656-C43FCA99F059}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>confirmpass</t>
   </si>
   <si>
-    <t>remark</t>
-  </si>
-  <si>
     <t>wk@g.com</t>
   </si>
   <si>
@@ -76,13 +73,16 @@
   </si>
   <si>
     <t>Valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expected </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,13 +98,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -120,9 +134,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -441,80 +456,83 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
     <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="E1" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1234567890</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>1234567890</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -529,5 +547,6 @@
     <hyperlink ref="D4" r:id="rId8" xr:uid="{B5D0C938-B63F-4D45-92EF-28F7641288FC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>